<commit_message>
UEN ACRA API fix
</commit_message>
<xml_diff>
--- a/Miscellaneous/Testing Data.xlsx
+++ b/Miscellaneous/Testing Data.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\MTech\MR\mr_groupproject-master\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3823BB-C0E7-4C65-9CA7-40C127E0E24E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Test Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>UEN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -97,23 +91,35 @@
   <si>
     <t>Negative due to Operational Status</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200604346E</t>
+  </si>
+  <si>
+    <t>201626142G</t>
+  </si>
+  <si>
+    <t>KUDOS DATA PTE. LTD.</t>
+  </si>
+  <si>
+    <t>NATIONAL UNIVERSITY OF SINGAPORE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -122,7 +128,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -163,11 +169,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -228,7 +236,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -263,7 +271,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -440,33 +448,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -495,20 +502,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>1000000</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>350000</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>2000</v>
       </c>
       <c r="F2" s="3">
@@ -517,27 +524,28 @@
       <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="3">
-        <v>12345678</v>
+      <c r="H2" s="3" t="str">
+        <f>A2</f>
+        <v>53272992K</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>1000000</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>350000</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>2000</v>
       </c>
       <c r="F3" s="3">
@@ -546,27 +554,28 @@
       <c r="G3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="3">
-        <v>12345678</v>
+      <c r="H3" s="3" t="str">
+        <f t="shared" ref="H3:H5" si="0">A3</f>
+        <v>53272992K</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>-100000</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <v>1000</v>
       </c>
       <c r="F4" s="3">
@@ -575,27 +584,28 @@
       <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="3">
-        <v>12345678</v>
+      <c r="H4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>53272992K</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>100000</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>35000</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>50</v>
       </c>
       <c r="F5" s="3">
@@ -604,11 +614,75 @@
       <c r="G5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="3">
-        <v>12345678</v>
+      <c r="H5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>53272992K</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D7" s="4">
+        <v>100000000</v>
+      </c>
+      <c r="E7" s="4">
+        <v>14000</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2008</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>10000</v>
+      </c>
+      <c r="E8" s="4">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2016</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>